<commit_message>
updated tables and cleaning to include armor materials
</commit_message>
<xml_diff>
--- a/raw_data/armour.xlsx
+++ b/raw_data/armour.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmaj\Documents\Games\Valheim\valheim_app\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB74C743-E9DB-4EE2-8B2D-2E1CBB3FC766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4DA2C9-1AA8-4604-8EAD-DA5331A4CD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{5052F365-B2B0-403D-8A0A-41E289D92662}"/>
+    <workbookView xWindow="19090" yWindow="-40" windowWidth="19420" windowHeight="10300" xr2:uid="{5052F365-B2B0-403D-8A0A-41E289D92662}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="62">
   <si>
     <t>item</t>
   </si>
@@ -63,9 +63,6 @@
     <t>other</t>
   </si>
   <si>
-    <t>cape of odin</t>
-  </si>
-  <si>
     <t>upgrade level</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
   </si>
   <si>
     <t>midsummer crown</t>
-  </si>
-  <si>
-    <t>hood of odin</t>
   </si>
   <si>
     <t>leather helmet</t>
@@ -582,11 +576,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1F69E8-11F4-4E9E-954F-E30D200E3A5D}">
-  <dimension ref="A1:I144"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I145" sqref="I145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O95" sqref="O95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,12 +615,12 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -640,7 +634,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -654,7 +648,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -668,7 +662,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -687,6 +681,9 @@
       <c r="B6">
         <v>1</v>
       </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
       <c r="F6">
         <v>4</v>
       </c>
@@ -701,6 +698,9 @@
       <c r="B7">
         <v>2</v>
       </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
       <c r="F7">
         <v>4</v>
       </c>
@@ -715,6 +715,9 @@
       <c r="B8">
         <v>3</v>
       </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
       <c r="F8">
         <v>4</v>
       </c>
@@ -729,6 +732,9 @@
       <c r="B9">
         <v>4</v>
       </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
       <c r="F9">
         <v>4</v>
       </c>
@@ -738,13 +744,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>12</v>
+      <c r="C10" t="s">
+        <v>15</v>
       </c>
       <c r="F10">
         <v>4</v>
@@ -755,13 +761,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
-        <v>12</v>
+      <c r="C11" t="s">
+        <v>15</v>
       </c>
       <c r="F11">
         <v>4</v>
@@ -772,13 +778,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
-        <v>12</v>
+      <c r="C12" t="s">
+        <v>15</v>
       </c>
       <c r="F12">
         <v>4</v>
@@ -789,13 +795,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="E13" t="s">
-        <v>12</v>
+      <c r="C13" t="s">
+        <v>15</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -806,13 +812,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>15</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -823,13 +829,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
         <v>15</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
       </c>
       <c r="F15">
         <v>4</v>
@@ -840,13 +846,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
         <v>15</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
       </c>
       <c r="F16">
         <v>4</v>
@@ -857,13 +863,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
         <v>15</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -879,9 +885,6 @@
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
       <c r="F18">
         <v>4</v>
       </c>
@@ -896,9 +899,6 @@
       <c r="B19">
         <v>2</v>
       </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
       <c r="F19">
         <v>4</v>
       </c>
@@ -913,9 +913,6 @@
       <c r="B20">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
       <c r="F20">
         <v>4</v>
       </c>
@@ -930,9 +927,6 @@
       <c r="B21">
         <v>4</v>
       </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
       <c r="F21">
         <v>4</v>
       </c>
@@ -947,8 +941,14 @@
       <c r="B22">
         <v>1</v>
       </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
       <c r="F22">
         <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>19</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -961,8 +961,14 @@
       <c r="B23">
         <v>2</v>
       </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
       <c r="F23">
         <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>19</v>
       </c>
       <c r="I23">
         <v>2</v>
@@ -970,70 +976,58 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F26">
-        <v>4</v>
-      </c>
-      <c r="H26" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F27">
-        <v>4</v>
-      </c>
-      <c r="H27" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1041,13 +1035,13 @@
         <v>21</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1055,7 +1049,10 @@
         <v>22</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1069,7 +1066,10 @@
         <v>22</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1083,7 +1083,10 @@
         <v>22</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1097,7 +1100,10 @@
         <v>22</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1111,10 +1117,10 @@
         <v>23</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -1125,10 +1131,10 @@
         <v>23</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I34">
         <v>2</v>
@@ -1139,10 +1145,10 @@
         <v>23</v>
       </c>
       <c r="B35">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I35">
         <v>3</v>
@@ -1153,10 +1159,10 @@
         <v>23</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I36">
         <v>4</v>
@@ -1167,13 +1173,19 @@
         <v>24</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -1184,13 +1196,19 @@
         <v>24</v>
       </c>
       <c r="B38">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" t="s">
+        <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I38">
         <v>2</v>
@@ -1201,13 +1219,19 @@
         <v>24</v>
       </c>
       <c r="B39">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" t="s">
+        <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I39">
         <v>3</v>
@@ -1218,13 +1242,19 @@
         <v>24</v>
       </c>
       <c r="B40">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" t="s">
+        <v>26</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I40">
         <v>4</v>
@@ -1232,10 +1262,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F41">
         <v>3</v>
@@ -1246,10 +1276,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B42">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F42">
         <v>3</v>
@@ -1260,10 +1290,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B43">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F43">
         <v>3</v>
@@ -1274,10 +1304,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B44">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F44">
         <v>3</v>
@@ -1288,22 +1318,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B45">
-        <v>8</v>
-      </c>
-      <c r="C45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D45" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F45">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0.03</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -1311,22 +1338,16 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B46">
-        <v>10</v>
-      </c>
-      <c r="C46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D46" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I46">
         <v>2</v>
@@ -1334,22 +1355,16 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B47">
-        <v>12</v>
-      </c>
-      <c r="C47" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E47" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I47">
         <v>3</v>
@@ -1357,22 +1372,16 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B48">
-        <v>14</v>
-      </c>
-      <c r="C48" t="s">
-        <v>27</v>
-      </c>
-      <c r="D48" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I48">
         <v>4</v>
@@ -1380,10 +1389,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B49">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F49">
         <v>3</v>
@@ -1394,10 +1403,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B50">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F50">
         <v>3</v>
@@ -1408,10 +1417,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B51">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F51">
         <v>3</v>
@@ -1422,10 +1431,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B52">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F52">
         <v>3</v>
@@ -1436,19 +1445,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B53">
-        <v>10</v>
-      </c>
-      <c r="E53" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F53">
-        <v>1</v>
-      </c>
-      <c r="G53" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="I53">
         <v>1</v>
@@ -1456,16 +1459,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B54">
-        <v>12</v>
-      </c>
-      <c r="E54" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I54">
         <v>2</v>
@@ -1473,16 +1473,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B55">
-        <v>14</v>
-      </c>
-      <c r="E55" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I55">
         <v>3</v>
@@ -1490,16 +1487,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56">
         <v>32</v>
       </c>
-      <c r="B56">
-        <v>16</v>
-      </c>
-      <c r="E56" t="s">
-        <v>33</v>
-      </c>
       <c r="F56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I56">
         <v>4</v>
@@ -1510,10 +1504,13 @@
         <v>34</v>
       </c>
       <c r="B57">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F57">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>35</v>
       </c>
       <c r="I57">
         <v>1</v>
@@ -1524,10 +1521,13 @@
         <v>34</v>
       </c>
       <c r="B58">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F58">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>35</v>
       </c>
       <c r="I58">
         <v>2</v>
@@ -1535,41 +1535,41 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B59">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F59">
         <v>3</v>
       </c>
       <c r="I59">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60">
         <v>34</v>
       </c>
-      <c r="B60">
-        <v>26</v>
-      </c>
       <c r="F60">
         <v>3</v>
       </c>
       <c r="I60">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B61">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I61">
         <v>1</v>
@@ -1577,13 +1577,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B62">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="F62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I62">
         <v>2</v>
@@ -1591,75 +1591,72 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B63">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F63">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I63">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B64">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F64">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I64">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B65">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F65">
-        <v>1</v>
-      </c>
-      <c r="H65" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="I65">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B66">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F66">
-        <v>1</v>
-      </c>
-      <c r="H66" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="I66">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B67">
-        <v>32</v>
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>11</v>
       </c>
       <c r="F67">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I67">
         <v>1</v>
@@ -1667,13 +1664,16 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B68">
-        <v>34</v>
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>11</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I68">
         <v>2</v>
@@ -1684,13 +1684,16 @@
         <v>39</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
       </c>
       <c r="F69">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I69">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -1698,13 +1701,16 @@
         <v>39</v>
       </c>
       <c r="B70">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
       </c>
       <c r="F70">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I70">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -1712,10 +1718,13 @@
         <v>40</v>
       </c>
       <c r="B71">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F71">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G71" s="2">
+        <v>-0.05</v>
       </c>
       <c r="I71">
         <v>1</v>
@@ -1726,10 +1735,13 @@
         <v>40</v>
       </c>
       <c r="B72">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F72">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G72" s="2">
+        <v>-0.05</v>
       </c>
       <c r="I72">
         <v>2</v>
@@ -1740,10 +1752,13 @@
         <v>40</v>
       </c>
       <c r="B73">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F73">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G73" s="2">
+        <v>-0.05</v>
       </c>
       <c r="I73">
         <v>3</v>
@@ -1754,10 +1769,13 @@
         <v>40</v>
       </c>
       <c r="B74">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F74">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G74" s="2">
+        <v>-0.05</v>
       </c>
       <c r="I74">
         <v>4</v>
@@ -1768,13 +1786,22 @@
         <v>41</v>
       </c>
       <c r="B75">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75" t="s">
+        <v>26</v>
       </c>
       <c r="E75" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F75">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G75" s="2">
+        <v>-0.02</v>
       </c>
       <c r="I75">
         <v>1</v>
@@ -1785,13 +1812,22 @@
         <v>41</v>
       </c>
       <c r="B76">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="C76" t="s">
+        <v>42</v>
+      </c>
+      <c r="D76" t="s">
+        <v>26</v>
       </c>
       <c r="E76" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F76">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G76" s="2">
+        <v>-0.02</v>
       </c>
       <c r="I76">
         <v>2</v>
@@ -1802,13 +1838,22 @@
         <v>41</v>
       </c>
       <c r="B77">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C77" t="s">
+        <v>42</v>
+      </c>
+      <c r="D77" t="s">
+        <v>26</v>
       </c>
       <c r="E77" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F77">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G77" s="2">
+        <v>-0.02</v>
       </c>
       <c r="I77">
         <v>3</v>
@@ -1819,13 +1864,22 @@
         <v>41</v>
       </c>
       <c r="B78">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C78" t="s">
+        <v>42</v>
+      </c>
+      <c r="D78" t="s">
+        <v>26</v>
       </c>
       <c r="E78" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F78">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G78" s="2">
+        <v>-0.02</v>
       </c>
       <c r="I78">
         <v>4</v>
@@ -1833,13 +1887,13 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B79">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F79">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G79" s="2">
         <v>-0.05</v>
@@ -1850,13 +1904,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B80">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F80">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G80" s="2">
         <v>-0.05</v>
@@ -1867,13 +1921,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B81">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F81">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G81" s="2">
         <v>-0.05</v>
@@ -1884,13 +1938,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B82">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F82">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G82" s="2">
         <v>-0.05</v>
@@ -1901,25 +1955,22 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B83">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C83" t="s">
-        <v>44</v>
-      </c>
-      <c r="D83" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E83" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F83">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G83" s="2">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I83">
         <v>1</v>
@@ -1927,25 +1978,22 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B84">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>44</v>
-      </c>
-      <c r="D84" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E84" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F84">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G84" s="2">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I84">
         <v>2</v>
@@ -1953,25 +2001,22 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B85">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C85" t="s">
-        <v>44</v>
-      </c>
-      <c r="D85" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E85" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F85">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G85" s="2">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I85">
         <v>3</v>
@@ -1979,25 +2024,22 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B86">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C86" t="s">
-        <v>44</v>
-      </c>
-      <c r="D86" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E86" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F86">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G86" s="2">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I86">
         <v>4</v>
@@ -2008,7 +2050,10 @@
         <v>45</v>
       </c>
       <c r="B87">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="C87" t="s">
+        <v>15</v>
       </c>
       <c r="F87">
         <v>15</v>
@@ -2025,7 +2070,10 @@
         <v>45</v>
       </c>
       <c r="B88">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="C88" t="s">
+        <v>15</v>
       </c>
       <c r="F88">
         <v>15</v>
@@ -2042,7 +2090,10 @@
         <v>45</v>
       </c>
       <c r="B89">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="C89" t="s">
+        <v>15</v>
       </c>
       <c r="F89">
         <v>15</v>
@@ -2059,7 +2110,10 @@
         <v>45</v>
       </c>
       <c r="B90">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="C90" t="s">
+        <v>15</v>
       </c>
       <c r="F90">
         <v>15</v>
@@ -2076,19 +2130,13 @@
         <v>46</v>
       </c>
       <c r="B91">
-        <v>10</v>
-      </c>
-      <c r="C91" t="s">
-        <v>28</v>
-      </c>
-      <c r="E91" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F91">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G91" s="2">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="I91">
         <v>1</v>
@@ -2099,19 +2147,13 @@
         <v>46</v>
       </c>
       <c r="B92">
-        <v>12</v>
-      </c>
-      <c r="C92" t="s">
         <v>28</v>
       </c>
-      <c r="E92" t="s">
-        <v>33</v>
-      </c>
       <c r="F92">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G92" s="2">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="I92">
         <v>2</v>
@@ -2122,19 +2164,13 @@
         <v>46</v>
       </c>
       <c r="B93">
-        <v>14</v>
-      </c>
-      <c r="C93" t="s">
-        <v>28</v>
-      </c>
-      <c r="E93" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F93">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G93" s="2">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="I93">
         <v>3</v>
@@ -2145,19 +2181,13 @@
         <v>46</v>
       </c>
       <c r="B94">
-        <v>16</v>
-      </c>
-      <c r="C94" t="s">
-        <v>28</v>
-      </c>
-      <c r="E94" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F94">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G94" s="2">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="I94">
         <v>4</v>
@@ -2168,16 +2198,16 @@
         <v>47</v>
       </c>
       <c r="B95">
-        <v>20</v>
-      </c>
-      <c r="C95" t="s">
         <v>16</v>
       </c>
       <c r="F95">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G95" s="2">
-        <v>-0.05</v>
+        <v>-0.02</v>
+      </c>
+      <c r="H95" t="s">
+        <v>48</v>
       </c>
       <c r="I95">
         <v>1</v>
@@ -2188,16 +2218,16 @@
         <v>47</v>
       </c>
       <c r="B96">
-        <v>22</v>
-      </c>
-      <c r="C96" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F96">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G96" s="2">
-        <v>-0.05</v>
+        <v>-0.02</v>
+      </c>
+      <c r="H96" t="s">
+        <v>48</v>
       </c>
       <c r="I96">
         <v>2</v>
@@ -2205,56 +2235,47 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B97">
-        <v>24</v>
-      </c>
-      <c r="C97" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F97">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G97" s="2">
         <v>-0.05</v>
       </c>
       <c r="I97">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B98">
-        <v>26</v>
-      </c>
-      <c r="C98" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F98">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G98" s="2">
         <v>-0.05</v>
       </c>
       <c r="I98">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B99">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F99">
-        <v>10</v>
-      </c>
-      <c r="G99" s="2">
-        <v>-0.05</v>
+        <v>2</v>
       </c>
       <c r="I99">
         <v>1</v>
@@ -2262,16 +2283,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B100">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="F100">
-        <v>10</v>
-      </c>
-      <c r="G100" s="2">
-        <v>-0.05</v>
+        <v>2</v>
       </c>
       <c r="I100">
         <v>2</v>
@@ -2279,90 +2297,72 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B101">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F101">
-        <v>10</v>
-      </c>
-      <c r="G101" s="2">
-        <v>-0.05</v>
+        <v>5</v>
       </c>
       <c r="I101">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B102">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F102">
-        <v>10</v>
-      </c>
-      <c r="G102" s="2">
-        <v>-0.05</v>
+        <v>5</v>
       </c>
       <c r="I102">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B103">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F103">
         <v>5</v>
       </c>
-      <c r="G103" s="2">
-        <v>-0.02</v>
-      </c>
-      <c r="H103" t="s">
-        <v>50</v>
-      </c>
       <c r="I103">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B104">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F104">
         <v>5</v>
       </c>
-      <c r="G104" s="2">
-        <v>-0.02</v>
-      </c>
-      <c r="H104" t="s">
-        <v>50</v>
-      </c>
       <c r="I104">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B105">
-        <v>32</v>
+        <v>6</v>
+      </c>
+      <c r="E105" t="s">
+        <v>11</v>
       </c>
       <c r="F105">
-        <v>10</v>
-      </c>
-      <c r="G105" s="2">
-        <v>-0.05</v>
+        <v>5</v>
       </c>
       <c r="I105">
         <v>1</v>
@@ -2370,16 +2370,16 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B106">
-        <v>34</v>
+        <v>8</v>
+      </c>
+      <c r="E106" t="s">
+        <v>11</v>
       </c>
       <c r="F106">
-        <v>10</v>
-      </c>
-      <c r="G106" s="2">
-        <v>-0.05</v>
+        <v>5</v>
       </c>
       <c r="I106">
         <v>2</v>
@@ -2390,13 +2390,16 @@
         <v>52</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="E107" t="s">
+        <v>11</v>
       </c>
       <c r="F107">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I107">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -2404,13 +2407,16 @@
         <v>52</v>
       </c>
       <c r="B108">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="E108" t="s">
+        <v>11</v>
       </c>
       <c r="F108">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I108">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -2418,10 +2424,13 @@
         <v>53</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F109">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G109" s="2">
+        <v>-0.05</v>
       </c>
       <c r="I109">
         <v>1</v>
@@ -2432,10 +2441,13 @@
         <v>53</v>
       </c>
       <c r="B110">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F110">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G110" s="2">
+        <v>-0.05</v>
       </c>
       <c r="I110">
         <v>2</v>
@@ -2446,10 +2458,13 @@
         <v>53</v>
       </c>
       <c r="B111">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F111">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G111" s="2">
+        <v>-0.05</v>
       </c>
       <c r="I111">
         <v>3</v>
@@ -2460,10 +2475,13 @@
         <v>53</v>
       </c>
       <c r="B112">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F112">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G112" s="2">
+        <v>-0.05</v>
       </c>
       <c r="I112">
         <v>4</v>
@@ -2474,13 +2492,19 @@
         <v>54</v>
       </c>
       <c r="B113">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D113" t="s">
+        <v>26</v>
       </c>
       <c r="E113" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F113">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G113" s="2">
+        <v>-0.02</v>
       </c>
       <c r="I113">
         <v>1</v>
@@ -2491,13 +2515,19 @@
         <v>54</v>
       </c>
       <c r="B114">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D114" t="s">
+        <v>26</v>
       </c>
       <c r="E114" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F114">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G114" s="2">
+        <v>-0.02</v>
       </c>
       <c r="I114">
         <v>2</v>
@@ -2508,13 +2538,19 @@
         <v>54</v>
       </c>
       <c r="B115">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D115" t="s">
+        <v>26</v>
       </c>
       <c r="E115" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F115">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G115" s="2">
+        <v>-0.02</v>
       </c>
       <c r="I115">
         <v>3</v>
@@ -2525,13 +2561,19 @@
         <v>54</v>
       </c>
       <c r="B116">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="D116" t="s">
+        <v>26</v>
       </c>
       <c r="E116" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F116">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G116" s="2">
+        <v>-0.02</v>
       </c>
       <c r="I116">
         <v>4</v>
@@ -2542,10 +2584,10 @@
         <v>55</v>
       </c>
       <c r="B117">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F117">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G117" s="2">
         <v>-0.05</v>
@@ -2559,10 +2601,10 @@
         <v>55</v>
       </c>
       <c r="B118">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F118">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G118" s="2">
         <v>-0.05</v>
@@ -2576,10 +2618,10 @@
         <v>55</v>
       </c>
       <c r="B119">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F119">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G119" s="2">
         <v>-0.05</v>
@@ -2593,10 +2635,10 @@
         <v>55</v>
       </c>
       <c r="B120">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F120">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G120" s="2">
         <v>-0.05</v>
@@ -2610,19 +2652,19 @@
         <v>56</v>
       </c>
       <c r="B121">
-        <v>8</v>
-      </c>
-      <c r="D121" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="C121" t="s">
+        <v>26</v>
       </c>
       <c r="E121" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F121">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G121" s="2">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I121">
         <v>1</v>
@@ -2633,19 +2675,19 @@
         <v>56</v>
       </c>
       <c r="B122">
-        <v>10</v>
-      </c>
-      <c r="D122" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="C122" t="s">
+        <v>26</v>
       </c>
       <c r="E122" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F122">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G122" s="2">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I122">
         <v>2</v>
@@ -2656,19 +2698,19 @@
         <v>56</v>
       </c>
       <c r="B123">
-        <v>12</v>
-      </c>
-      <c r="D123" t="s">
-        <v>28</v>
+        <v>14</v>
+      </c>
+      <c r="C123" t="s">
+        <v>26</v>
       </c>
       <c r="E123" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F123">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G123" s="2">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I123">
         <v>3</v>
@@ -2679,19 +2721,19 @@
         <v>56</v>
       </c>
       <c r="B124">
-        <v>14</v>
-      </c>
-      <c r="D124" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="C124" t="s">
+        <v>26</v>
       </c>
       <c r="E124" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F124">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G124" s="2">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I124">
         <v>4</v>
@@ -2702,7 +2744,7 @@
         <v>57</v>
       </c>
       <c r="B125">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F125">
         <v>15</v>
@@ -2719,7 +2761,7 @@
         <v>57</v>
       </c>
       <c r="B126">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F126">
         <v>15</v>
@@ -2736,7 +2778,7 @@
         <v>57</v>
       </c>
       <c r="B127">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F127">
         <v>15</v>
@@ -2753,7 +2795,7 @@
         <v>57</v>
       </c>
       <c r="B128">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F128">
         <v>15</v>
@@ -2770,19 +2812,13 @@
         <v>58</v>
       </c>
       <c r="B129">
-        <v>10</v>
-      </c>
-      <c r="C129" t="s">
-        <v>28</v>
-      </c>
-      <c r="E129" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F129">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G129" s="2">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="I129">
         <v>1</v>
@@ -2793,19 +2829,13 @@
         <v>58</v>
       </c>
       <c r="B130">
-        <v>12</v>
-      </c>
-      <c r="C130" t="s">
         <v>28</v>
       </c>
-      <c r="E130" t="s">
-        <v>33</v>
-      </c>
       <c r="F130">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G130" s="2">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="I130">
         <v>2</v>
@@ -2816,19 +2846,13 @@
         <v>58</v>
       </c>
       <c r="B131">
-        <v>14</v>
-      </c>
-      <c r="C131" t="s">
-        <v>28</v>
-      </c>
-      <c r="E131" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F131">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G131" s="2">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="I131">
         <v>3</v>
@@ -2839,19 +2863,13 @@
         <v>58</v>
       </c>
       <c r="B132">
-        <v>16</v>
-      </c>
-      <c r="C132" t="s">
-        <v>28</v>
-      </c>
-      <c r="E132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F132">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G132" s="2">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="I132">
         <v>4</v>
@@ -2862,13 +2880,16 @@
         <v>59</v>
       </c>
       <c r="B133">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F133">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G133" s="2">
-        <v>-0.05</v>
+        <v>-0.02</v>
+      </c>
+      <c r="H133" t="s">
+        <v>48</v>
       </c>
       <c r="I133">
         <v>1</v>
@@ -2879,13 +2900,13 @@
         <v>59</v>
       </c>
       <c r="B134">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F134">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G134" s="2">
-        <v>-0.05</v>
+        <v>-0.02</v>
       </c>
       <c r="I134">
         <v>2</v>
@@ -2893,174 +2914,35 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B135">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F135">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G135" s="2">
         <v>-0.05</v>
       </c>
       <c r="I135">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B136">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F136">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G136" s="2">
         <v>-0.05</v>
       </c>
       <c r="I136">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>60</v>
-      </c>
-      <c r="B137">
-        <v>26</v>
-      </c>
-      <c r="F137">
-        <v>10</v>
-      </c>
-      <c r="G137" s="2">
-        <v>-0.05</v>
-      </c>
-      <c r="I137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>60</v>
-      </c>
-      <c r="B138">
-        <v>28</v>
-      </c>
-      <c r="F138">
-        <v>10</v>
-      </c>
-      <c r="G138" s="2">
-        <v>-0.05</v>
-      </c>
-      <c r="I138">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>60</v>
-      </c>
-      <c r="B139">
-        <v>30</v>
-      </c>
-      <c r="F139">
-        <v>10</v>
-      </c>
-      <c r="G139" s="2">
-        <v>-0.05</v>
-      </c>
-      <c r="I139">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>60</v>
-      </c>
-      <c r="B140">
-        <v>32</v>
-      </c>
-      <c r="F140">
-        <v>10</v>
-      </c>
-      <c r="G140" s="2">
-        <v>-0.05</v>
-      </c>
-      <c r="I140">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>61</v>
-      </c>
-      <c r="B141">
-        <v>16</v>
-      </c>
-      <c r="F141">
-        <v>5</v>
-      </c>
-      <c r="G141" s="2">
-        <v>-0.02</v>
-      </c>
-      <c r="H141" t="s">
-        <v>50</v>
-      </c>
-      <c r="I141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>61</v>
-      </c>
-      <c r="B142">
-        <v>18</v>
-      </c>
-      <c r="F142">
-        <v>5</v>
-      </c>
-      <c r="G142" s="2">
-        <v>-0.02</v>
-      </c>
-      <c r="I142">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>62</v>
-      </c>
-      <c r="B143">
-        <v>32</v>
-      </c>
-      <c r="F143">
-        <v>10</v>
-      </c>
-      <c r="G143" s="2">
-        <v>-0.05</v>
-      </c>
-      <c r="I143">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>62</v>
-      </c>
-      <c r="B144">
-        <v>34</v>
-      </c>
-      <c r="F144">
-        <v>10</v>
-      </c>
-      <c r="G144" s="2">
-        <v>-0.05</v>
-      </c>
-      <c r="I144">
         <v>2</v>
       </c>
     </row>
@@ -3073,7 +2955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137808DB-2787-4D0A-A408-2A0257306D55}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3084,31 +2966,31 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>